<commit_message>
AUTO FROM work 06.05.2024 12:39:43,26
</commit_message>
<xml_diff>
--- a/бесценный/Книга1.xlsx
+++ b/бесценный/Книга1.xlsx
@@ -268,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -323,15 +323,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -343,6 +334,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -646,18 +652,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="9.140625" style="25"/>
+    <col min="6" max="6" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>14</v>
       </c>
@@ -671,7 +677,7 @@
       <c r="E1">
         <v>3.52</v>
       </c>
-      <c r="F1" s="23">
+      <c r="F1" s="20">
         <f>17/500*97</f>
         <v>3.298</v>
       </c>
@@ -682,8 +688,11 @@
         <f>20*3988/100</f>
         <v>797.6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="29">
+        <v>51.36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>12</v>
       </c>
@@ -691,13 +700,13 @@
         <v>0.3</v>
       </c>
       <c r="C2" s="2">
-        <f t="shared" ref="C2:C32" si="0">B2*A2</f>
+        <f t="shared" ref="C2:C31" si="0">B2*A2</f>
         <v>3.5999999999999996</v>
       </c>
       <c r="E2">
         <v>2.1</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>2.15</v>
       </c>
       <c r="H2">
@@ -707,8 +716,15 @@
         <f>48.59/3529.2*100</f>
         <v>1.3767992746231443</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="25">
+        <v>785.02</v>
+      </c>
+      <c r="O2">
+        <f>51.36/4001</f>
+        <v>1.2836790802299426E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>9</v>
       </c>
@@ -722,7 +738,7 @@
       <c r="E3">
         <v>29.9</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>30.5</v>
       </c>
       <c r="H3">
@@ -731,8 +747,11 @@
       <c r="I3">
         <v>22.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="25">
+        <v>266.91000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>8</v>
       </c>
@@ -746,7 +765,7 @@
       <c r="E4">
         <v>35.520000000000003</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>35.950000000000003</v>
       </c>
       <c r="H4">
@@ -756,8 +775,11 @@
         <f>F9/F15*100</f>
         <v>7.5422191998186561</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K4" s="25">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>5</v>
       </c>
@@ -771,9 +793,12 @@
       <c r="E5">
         <v>11.51</v>
       </c>
-      <c r="F5" s="24">
-        <f>0.32*(98.55*0.4+0.27*0.35)</f>
-        <v>12.644639999999999</v>
+      <c r="F5" s="21">
+        <f>0.39*(98.55*0.4+0.27*0.35)</f>
+        <v>15.410655</v>
+      </c>
+      <c r="G5">
+        <v>12.64</v>
       </c>
       <c r="H5">
         <v>0.17</v>
@@ -782,8 +807,11 @@
         <f>F13/F15*100</f>
         <v>0.19126147568854132</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="25">
+        <v>2431.4499999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -797,9 +825,13 @@
       <c r="E6">
         <v>47.03</v>
       </c>
-      <c r="F6" s="25">
+      <c r="F6" s="22">
         <f>35.95+12.64</f>
         <v>48.59</v>
+      </c>
+      <c r="G6" s="19">
+        <f xml:space="preserve"> 35.95 + 15.41</f>
+        <v>51.36</v>
       </c>
       <c r="H6">
         <v>70.209999999999994</v>
@@ -808,8 +840,12 @@
         <f>F10/F15*100</f>
         <v>68.707780800181339</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <f>SUM(K1:K5)</f>
+        <v>3541.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -823,8 +859,11 @@
       <c r="E7">
         <v>89.64</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="22">
         <v>98.55</v>
+      </c>
+      <c r="G7">
+        <v>98.82</v>
       </c>
       <c r="H7">
         <v>0.1</v>
@@ -834,7 +873,7 @@
         <v>1.015337679705784E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -848,18 +887,21 @@
       <c r="E8">
         <v>703.83</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="22">
         <v>782.87</v>
+      </c>
+      <c r="G8">
+        <v>785.02</v>
       </c>
       <c r="H8">
         <v>0.26</v>
       </c>
       <c r="I8">
-        <f>F5/F19*100</f>
-        <v>0.26422266800401201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f>F5/G19*100</f>
+        <v>0.32090288363027564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -873,18 +915,21 @@
       <c r="E9">
         <v>239.3</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="22">
         <v>266.18</v>
+      </c>
+      <c r="G9">
+        <v>266.91000000000003</v>
       </c>
       <c r="H9">
         <v>0.74</v>
       </c>
       <c r="I9">
-        <f>F15/F19</f>
-        <v>0.73746238716148438</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <f>G15/G19</f>
+        <v>0.73746012310819031</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -898,12 +943,22 @@
       <c r="E10">
         <v>2346.12</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="22">
         <f>350*F14/100</f>
         <v>2424.8349999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <f>350*G14/100</f>
+        <v>2431.4500000000003</v>
+      </c>
+      <c r="H10">
+        <v>0.1</v>
+      </c>
+      <c r="I10">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>2</v>
       </c>
@@ -917,12 +972,12 @@
       <c r="E11">
         <v>1854.72</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="22">
         <f>2016*(0.93)</f>
         <v>1874.88</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>3</v>
       </c>
@@ -936,12 +991,15 @@
       <c r="E12">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F12" s="25">
+      <c r="F12" s="22">
         <f>98.55/F11</f>
         <v>5.2563364055299537E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>6</v>
       </c>
@@ -955,12 +1013,12 @@
       <c r="E13">
         <v>5.52</v>
       </c>
-      <c r="F13" s="25">
+      <c r="F13" s="22">
         <f>1350*0.05/10</f>
         <v>6.75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>2</v>
       </c>
@@ -974,11 +1032,14 @@
       <c r="E14">
         <v>617.4</v>
       </c>
-      <c r="F14" s="25">
+      <c r="F14" s="22">
         <v>692.81</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>694.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -992,11 +1053,15 @@
       <c r="E15">
         <v>3341.8</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="19">
         <v>3529.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="19">
+        <f xml:space="preserve"> 51.36+ 785.02+266.91+6.75+2431.45</f>
+        <v>3541.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>6</v>
       </c>
@@ -1010,9 +1075,13 @@
       <c r="E16">
         <v>401.02</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="22">
         <f>13*3529.2/100</f>
         <v>458.79599999999999</v>
+      </c>
+      <c r="G16">
+        <f>3541.5*13/100</f>
+        <v>460.39499999999998</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1029,9 +1098,13 @@
       <c r="E17">
         <v>3742.82</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="19">
         <f xml:space="preserve"> 3529.2 + 458.8</f>
         <v>3988</v>
+      </c>
+      <c r="G17" s="19">
+        <f xml:space="preserve"> 3541.5 + 460.4</f>
+        <v>4001.9</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1048,7 +1121,7 @@
       <c r="E18">
         <v>12</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="22">
         <v>13</v>
       </c>
     </row>
@@ -1066,9 +1139,13 @@
       <c r="E19">
         <v>4491.3999999999996</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="19">
         <f xml:space="preserve"> 3988+797.6</f>
         <v>4785.6000000000004</v>
+      </c>
+      <c r="G19" s="19">
+        <f xml:space="preserve"> 4001.9+800.38</f>
+        <v>4802.28</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1082,6 +1159,13 @@
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
+      <c r="F20" s="22">
+        <v>797.6</v>
+      </c>
+      <c r="G20">
+        <f>20*4001.9/100</f>
+        <v>800.38</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
@@ -1118,10 +1202,10 @@
         <f t="shared" si="0"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="E23" s="26">
+      <c r="E23" s="23">
         <v>1.38</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="23">
         <v>48.59</v>
       </c>
     </row>
@@ -1136,10 +1220,10 @@
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="24">
         <v>22.18</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="24">
         <v>782.87</v>
       </c>
     </row>
@@ -1154,10 +1238,10 @@
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="24">
         <v>7.54</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="24">
         <v>266.18</v>
       </c>
     </row>
@@ -1172,10 +1256,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="24">
         <v>0.19</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="24">
         <v>6.75</v>
       </c>
     </row>
@@ -1190,10 +1274,10 @@
         <f t="shared" si="0"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="24">
         <v>68.709999999999994</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="24">
         <v>2424.84</v>
       </c>
     </row>
@@ -1265,31 +1349,31 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
-      <c r="B33" s="19"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="16">
         <f>C34+C35</f>
         <v>98.82</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="17">
         <f>SUM(C1:C31)</f>
         <v>98.55</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="18">
         <f>C32</f>
         <v>0.27</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="22">
+      <c r="A38" s="19">
         <f>0.32*(98.55*0.4+0.27*0.35)</f>
         <v>12.644639999999999</v>
       </c>

</xml_diff>